<commit_message>
Per Capita Income Tables
</commit_message>
<xml_diff>
--- a/tidytuesday_week_19/airline_by_continent.xlsx
+++ b/tidytuesday_week_19/airline_by_continent.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="112">
   <si>
     <t>airline</t>
   </si>
@@ -222,6 +222,147 @@
   </si>
   <si>
     <t>Europe</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
   </si>
 </sst>
 </file>
@@ -536,471 +677,643 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>59</v>
+      </c>
+      <c r="C57" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>